<commit_message>
Notas da Lista 02 e da Prova 01 adicionadas
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53064bec2e33241/Desktop/dce692/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E2D40D8B-AFF5-4982-8D7D-E46FC4162430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{E2D40D8B-AFF5-4982-8D7D-E46FC4162430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FC6E815-FF2D-4077-B3C9-54E32A7456C4}"/>
   <bookViews>
     <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{E291B56F-1897-4A20-9954-4388617D9E19}"/>
   </bookViews>
   <sheets>
-    <sheet name="Listas" sheetId="1" r:id="rId1"/>
+    <sheet name="Provas" sheetId="2" r:id="rId1"/>
+    <sheet name="Listas" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>Matrícula</t>
   </si>
@@ -103,6 +104,21 @@
   </si>
   <si>
     <t>2016.1.08.023</t>
+  </si>
+  <si>
+    <t>Lista 03</t>
+  </si>
+  <si>
+    <t>Prova 01</t>
+  </si>
+  <si>
+    <t>As notas das provas variam entre 0 e 100</t>
+  </si>
+  <si>
+    <t>A nota de cada prova será multiplicada por 0.25 para fins de computação da nota final da disciplina</t>
+  </si>
+  <si>
+    <t>Prova 02</t>
   </si>
 </sst>
 </file>
@@ -151,10 +167,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,11 +484,253 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBACA92-77C3-4098-AB23-6C7B2EAEA915}">
+  <dimension ref="A1:J26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <f>(15+22+20+35)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>(15+25+20+25)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f>(12+23+20+25)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f>(19+16+20+35)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f>(16+25+18+25)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f>(15+25+20+25)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f>(10+22+15+25)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f>(19+16+20+25)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f>(8+25+20+25)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f>(13+24+20+35)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f>(8+25+15+30)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f>(15+24+20+25)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f>(12+23+20+35)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f>(16+25+20+35)</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f>(12+25+15+25)</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f>(10+15+25+25)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f>(13+23+20+25)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f>(15+25+20+25)</f>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f>(10+25+15+25)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f>(16+25+20+35)</f>
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9168A79-CAE1-418C-B1AD-8EE8954EBBCC}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,37 +739,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -523,13 +781,19 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <v>90</v>
+      </c>
+      <c r="C7">
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -539,6 +803,9 @@
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -547,6 +814,9 @@
       <c r="B9">
         <v>80</v>
       </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -555,6 +825,9 @@
       <c r="B10">
         <v>70</v>
       </c>
+      <c r="C10">
+        <v>80</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -563,6 +836,9 @@
       <c r="B11">
         <v>0</v>
       </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -571,6 +847,9 @@
       <c r="B12">
         <v>90</v>
       </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -579,6 +858,9 @@
       <c r="B13">
         <v>90</v>
       </c>
+      <c r="C13">
+        <v>95</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -587,6 +869,9 @@
       <c r="B14">
         <v>80</v>
       </c>
+      <c r="C14">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -595,6 +880,9 @@
       <c r="B15">
         <v>100</v>
       </c>
+      <c r="C15">
+        <v>85</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -603,85 +891,118 @@
       <c r="B16">
         <v>65</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>100</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <v>80</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
         <v>65</v>
+      </c>
+      <c r="C26">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Notas das listas 03 e 04
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d53064bec2e33241/Desktop/dce692/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{E2D40D8B-AFF5-4982-8D7D-E46FC4162430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FC6E815-FF2D-4077-B3C9-54E32A7456C4}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{E2D40D8B-AFF5-4982-8D7D-E46FC4162430}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{990EF2A9-F018-45C4-A169-811DADB42C08}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{E291B56F-1897-4A20-9954-4388617D9E19}"/>
+    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" activeTab="1" xr2:uid="{E291B56F-1897-4A20-9954-4388617D9E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Provas" sheetId="2" r:id="rId1"/>
     <sheet name="Listas" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Matrícula</t>
   </si>
@@ -119,6 +126,12 @@
   </si>
   <si>
     <t>Prova 02</t>
+  </si>
+  <si>
+    <t>Lista 04</t>
+  </si>
+  <si>
+    <t>Média final</t>
   </si>
 </sst>
 </file>
@@ -487,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DBACA92-77C3-4098-AB23-6C7B2EAEA915}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -729,13 +742,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9168A79-CAE1-418C-B1AD-8EE8954EBBCC}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -784,6 +798,12 @@
       <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -795,6 +815,16 @@
       <c r="C7">
         <v>85</v>
       </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <f>AVERAGE(B7:E7)</f>
+        <v>93.75</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -806,6 +836,16 @@
       <c r="C8">
         <v>100</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G26" si="0">AVERAGE(B8:E8)</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -817,6 +857,16 @@
       <c r="C9">
         <v>40</v>
       </c>
+      <c r="D9">
+        <v>90</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>57.5</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -828,6 +878,16 @@
       <c r="C10">
         <v>80</v>
       </c>
+      <c r="D10">
+        <v>80</v>
+      </c>
+      <c r="E10">
+        <v>85</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>78.75</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -839,6 +899,16 @@
       <c r="C11">
         <v>100</v>
       </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -850,6 +920,16 @@
       <c r="C12">
         <v>100</v>
       </c>
+      <c r="D12">
+        <v>90</v>
+      </c>
+      <c r="E12">
+        <v>99</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>94.75</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -861,6 +941,16 @@
       <c r="C13">
         <v>95</v>
       </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>46.25</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -872,6 +962,16 @@
       <c r="C14">
         <v>80</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -883,6 +983,16 @@
       <c r="C15">
         <v>85</v>
       </c>
+      <c r="D15">
+        <v>80</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>91.25</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -894,8 +1004,18 @@
       <c r="C16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>90</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>88.75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -905,8 +1025,18 @@
       <c r="C17">
         <v>95</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="0"/>
+        <v>48.75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -916,8 +1046,18 @@
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -927,8 +1067,18 @@
       <c r="C19">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>70</v>
+      </c>
+      <c r="E19">
+        <v>85</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -938,8 +1088,18 @@
       <c r="C20">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>90</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="0"/>
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -949,8 +1109,18 @@
       <c r="C21">
         <v>70</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>75</v>
+      </c>
+      <c r="E21">
+        <v>85</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="0"/>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -960,8 +1130,18 @@
       <c r="C22">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>85</v>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -971,8 +1151,18 @@
       <c r="C23">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>95</v>
+      </c>
+      <c r="E23">
+        <v>85</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>82.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -982,8 +1172,18 @@
       <c r="C24">
         <v>75</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>43.75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -993,8 +1193,18 @@
       <c r="C25">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1003,6 +1213,16 @@
       </c>
       <c r="C26">
         <v>95</v>
+      </c>
+      <c r="D26">
+        <v>90</v>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>87.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>